<commit_message>
Extent report & Assertions completed
</commit_message>
<xml_diff>
--- a/Mars_Task02/Mars_Task02/ExcelData/TestDataManageListings.xlsx
+++ b/Mars_Task02/Mars_Task02/ExcelData/TestDataManageListings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nikit\Mars_Task02\Mars_Task02\Mars_Task02\Mars_Task02\ExcelData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED30DDA7-39A6-4738-97BA-E63A91A17DAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CFC9A46-8E4C-4A7A-B8DE-FA75B7DA2049}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{65B866A7-7CF8-4914-B43D-1C2DF72F73CE}"/>
   </bookViews>
@@ -66,10 +66,10 @@
     <t>Web based application</t>
   </si>
   <si>
-    <t>08.00 PM</t>
-  </si>
-  <si>
     <t>Software Tester</t>
+  </si>
+  <si>
+    <t>08.00 AM</t>
   </si>
 </sst>
 </file>
@@ -451,7 +451,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -487,7 +487,7 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B2" t="s">
         <v>8</v>
@@ -496,13 +496,13 @@
         <v>9</v>
       </c>
       <c r="D2" s="4">
-        <v>45061</v>
+        <v>45092</v>
       </c>
       <c r="E2" s="4">
         <v>45153</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>7</v>

</xml_diff>